<commit_message>
added till heat map
</commit_message>
<xml_diff>
--- a/10_Data_Analysis/CONTENT FILES/data.xlsx
+++ b/10_Data_Analysis/CONTENT FILES/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Programming Studies\Tutedude\10_Data_Analysis\CONTENT FILES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17526C2-EBBE-425D-8792-BA1B18D25F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACCD4D3-3F55-433C-897E-9636207DA6D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5760" yWindow="12" windowWidth="17280" windowHeight="8880" xr2:uid="{81042238-8ECE-45D5-B980-E5B9C302240B}"/>
   </bookViews>
@@ -409,7 +409,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,7 +549,7 @@
         <v>20</v>
       </c>
       <c r="G6">
-        <v>84</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>